<commit_message>
Updated the github address on some files.
</commit_message>
<xml_diff>
--- a/FpML.V5r3.Applications/ExcelAPI/Spreadsheets/Bonds/BondAssets.xlsx
+++ b/FpML.V5r3.Applications/ExcelAPI/Spreadsheets/Bonds/BondAssets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\Visual Studio 2019\Projects\Highlander\FpML.V5r3.Applications\ExcelAPI\Spreadsheets\Bonds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B72D035-F006-4454-B452-E6A6AE362B15}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C41F9D6-62AE-47EF-9041-75D3035D8524}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3090" yWindow="1230" windowWidth="21600" windowHeight="13845" tabRatio="497" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4860" yWindow="690" windowWidth="23940" windowHeight="13845" tabRatio="497" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table of Contents" sheetId="5" r:id="rId1"/>
@@ -3072,7 +3072,7 @@
     <row r="49" spans="2:13">
       <c r="B49" s="98" t="str">
         <f ca="1">"Last Update "&amp;TEXT(TODAY(),"dd-mmm-yy")</f>
-        <v>Last Update 04-Jun-19</v>
+        <v>Last Update 24-Jun-19</v>
       </c>
       <c r="C49" s="91"/>
       <c r="D49" s="91"/>
@@ -3154,7 +3154,7 @@
       </c>
       <c r="C3" s="104">
         <f ca="1">NOW()</f>
-        <v>43620.688124768516</v>
+        <v>43640.48577013889</v>
       </c>
       <c r="D3" s="26"/>
       <c r="I3" t="str">
@@ -3168,7 +3168,7 @@
       </c>
       <c r="C4" s="106">
         <f ca="1">C3</f>
-        <v>43620.688124768516</v>
+        <v>43640.48577013889</v>
       </c>
       <c r="D4" s="26"/>
     </row>
@@ -3798,7 +3798,7 @@
   <dimension ref="A1:Z70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" outlineLevelCol="1"/>
@@ -3814,7 +3814,7 @@
     <col min="9" max="9" width="4.42578125" style="6" customWidth="1"/>
     <col min="10" max="10" width="24.140625" style="6" bestFit="1" customWidth="1" outlineLevel="1"/>
     <col min="11" max="11" width="11.42578125" style="6" bestFit="1" customWidth="1" outlineLevel="1"/>
-    <col min="12" max="12" width="7.140625" style="6" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="12" max="12" width="8.85546875" style="6" bestFit="1" customWidth="1" outlineLevel="1"/>
     <col min="13" max="13" width="14.42578125" style="6" bestFit="1" customWidth="1" outlineLevel="1"/>
     <col min="14" max="14" width="5.7109375" style="6" bestFit="1" customWidth="1" outlineLevel="1"/>
     <col min="15" max="15" width="5.42578125" style="6" bestFit="1" customWidth="1" outlineLevel="1"/>
@@ -3875,7 +3875,7 @@
     <row r="2" spans="1:26" ht="12" thickBot="1">
       <c r="A2" s="7" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.CreateSimpleBond(B2, B38, E2, F2, G2)</f>
-        <v>AUD-Bond-AGB.0.04.28/02/2022</v>
+        <v>AUD-Bond-AGB.0.04.20/03/2022</v>
       </c>
       <c r="B2" s="13" t="str">
         <f>C2&amp;"-Bond-"&amp;D2</f>
@@ -3889,7 +3889,7 @@
       </c>
       <c r="E2" s="83">
         <f ca="1">TODAY()+1000</f>
-        <v>44620</v>
+        <v>44640</v>
       </c>
       <c r="F2" s="36">
         <v>0.04</v>
@@ -3926,7 +3926,7 @@
     <row r="3" spans="1:26">
       <c r="A3" s="13" t="str">
         <f t="array" aca="1" ref="A3:A22" ca="1">_xll.HLV5r3.Financial.Cache.CreateSimpleBonds(B3:B22, $B$38, E3:E22, F3:F22, G3:G22)</f>
-        <v>AUD-Bond-AGB.0.04.1/06/2020</v>
+        <v>AUD-Bond-AGB.0.04.21/06/2020</v>
       </c>
       <c r="B3" s="13" t="str">
         <f>C3&amp;"-Bond-"&amp;D3</f>
@@ -3940,7 +3940,7 @@
       </c>
       <c r="E3" s="83">
         <f ca="1">TODAY()+363</f>
-        <v>43983</v>
+        <v>44003</v>
       </c>
       <c r="F3" s="36">
         <v>0.04</v>
@@ -3954,7 +3954,7 @@
       <c r="I3" s="9"/>
       <c r="J3" s="14" t="str">
         <f t="array" aca="1" ref="J3:X22" ca="1">_xll.HLV5r3.Financial.Cache.EvaluateMetricsForAssetSet($H$2:$H$7,$B$36, A3:A22, $B$38)</f>
-        <v>AUD-Bond-AGB.0.04.1/06/2020</v>
+        <v>AUD-Bond-AGB.0.04.21/06/2020</v>
       </c>
       <c r="K3" s="15" t="str">
         <f ca="1"/>
@@ -3978,7 +3978,7 @@
       </c>
       <c r="P3" s="117">
         <f ca="1"/>
-        <v>9.7348357975800652E-3</v>
+        <v>9.7337164492171183E-3</v>
       </c>
       <c r="Q3" s="16" t="str">
         <f ca="1"/>
@@ -4018,7 +4018,7 @@
     <row r="4" spans="1:26">
       <c r="A4" s="13" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.6/07/2021</v>
+        <v>AUD-Bond-AGB.0.04.26/07/2021</v>
       </c>
       <c r="B4" s="13" t="str">
         <f t="shared" ref="B4:B22" si="0">C4&amp;"-Bond-"&amp;D4</f>
@@ -4032,7 +4032,7 @@
       </c>
       <c r="E4" s="83">
         <f t="shared" ref="E4:E22" ca="1" si="1">E3+400</f>
-        <v>44383</v>
+        <v>44403</v>
       </c>
       <c r="F4" s="36">
         <v>0.04</v>
@@ -4046,7 +4046,7 @@
       <c r="I4" s="18"/>
       <c r="J4" s="19" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.6/07/2021</v>
+        <v>AUD-Bond-AGB.0.04.26/07/2021</v>
       </c>
       <c r="K4" s="10" t="str">
         <f ca="1"/>
@@ -4070,7 +4070,7 @@
       </c>
       <c r="P4" s="118">
         <f ca="1"/>
-        <v>2.3933118071269927E-2</v>
+        <v>2.3932000570792946E-2</v>
       </c>
       <c r="Q4" s="20" t="str">
         <f ca="1"/>
@@ -4110,7 +4110,7 @@
     <row r="5" spans="1:26">
       <c r="A5" s="13" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.10/08/2022</v>
+        <v>AUD-Bond-AGB.0.04.30/08/2022</v>
       </c>
       <c r="B5" s="13" t="str">
         <f t="shared" si="0"/>
@@ -4124,7 +4124,7 @@
       </c>
       <c r="E5" s="83">
         <f t="shared" ca="1" si="1"/>
-        <v>44783</v>
+        <v>44803</v>
       </c>
       <c r="F5" s="36">
         <v>0.04</v>
@@ -4138,7 +4138,7 @@
       <c r="I5" s="18"/>
       <c r="J5" s="19" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.10/08/2022</v>
+        <v>AUD-Bond-AGB.0.04.30/08/2022</v>
       </c>
       <c r="K5" s="10" t="str">
         <f ca="1"/>
@@ -4146,7 +4146,7 @@
       </c>
       <c r="L5" s="38">
         <f ca="1"/>
-        <v>1.0127720614331199</v>
+        <v>1.0128507778089599</v>
       </c>
       <c r="M5" s="10" t="str">
         <f ca="1"/>
@@ -4154,7 +4154,7 @@
       </c>
       <c r="N5" s="128">
         <f ca="1"/>
-        <v>101.25501295941307</v>
+        <v>101.26288287206106</v>
       </c>
       <c r="O5" s="10" t="str">
         <f ca="1"/>
@@ -4162,7 +4162,7 @@
       </c>
       <c r="P5" s="118">
         <f ca="1"/>
-        <v>3.2740001264981632E-2</v>
+        <v>3.2796514448903885E-2</v>
       </c>
       <c r="Q5" s="20" t="str">
         <f ca="1"/>
@@ -4202,7 +4202,7 @@
     <row r="6" spans="1:26">
       <c r="A6" s="13" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.14/09/2023</v>
+        <v>AUD-Bond-AGB.0.04.4/10/2023</v>
       </c>
       <c r="B6" s="13" t="str">
         <f t="shared" si="0"/>
@@ -4216,7 +4216,7 @@
       </c>
       <c r="E6" s="83">
         <f t="shared" ca="1" si="1"/>
-        <v>45183</v>
+        <v>45203</v>
       </c>
       <c r="F6" s="36">
         <v>0.04</v>
@@ -4228,7 +4228,7 @@
       <c r="I6" s="18"/>
       <c r="J6" s="19" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.14/09/2023</v>
+        <v>AUD-Bond-AGB.0.04.4/10/2023</v>
       </c>
       <c r="K6" s="10" t="str">
         <f ca="1"/>
@@ -4236,7 +4236,7 @@
       </c>
       <c r="L6" s="38">
         <f ca="1"/>
-        <v>1.00908131705403</v>
+        <v>1.0090219743548801</v>
       </c>
       <c r="M6" s="10" t="str">
         <f ca="1"/>
@@ -4244,7 +4244,7 @@
       </c>
       <c r="N6" s="128">
         <f ca="1"/>
-        <v>100.88601939791432</v>
+        <v>100.88008642839404</v>
       </c>
       <c r="O6" s="10" t="str">
         <f ca="1"/>
@@ -4252,7 +4252,7 @@
       </c>
       <c r="P6" s="118">
         <f ca="1"/>
-        <v>4.1219483287832544E-2</v>
+        <v>4.1191409225107611E-2</v>
       </c>
       <c r="Q6" s="20" t="str">
         <f ca="1"/>
@@ -4292,7 +4292,7 @@
     <row r="7" spans="1:26">
       <c r="A7" s="13" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.18/10/2024</v>
+        <v>AUD-Bond-AGB.0.04.7/11/2024</v>
       </c>
       <c r="B7" s="13" t="str">
         <f t="shared" si="0"/>
@@ -4306,7 +4306,7 @@
       </c>
       <c r="E7" s="83">
         <f t="shared" ca="1" si="1"/>
-        <v>45583</v>
+        <v>45603</v>
       </c>
       <c r="F7" s="36">
         <v>0.04</v>
@@ -4318,7 +4318,7 @@
       <c r="I7" s="18"/>
       <c r="J7" s="19" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.18/10/2024</v>
+        <v>AUD-Bond-AGB.0.04.7/11/2024</v>
       </c>
       <c r="K7" s="10" t="str">
         <f ca="1"/>
@@ -4326,7 +4326,7 @@
       </c>
       <c r="L7" s="38">
         <f ca="1"/>
-        <v>1.00531642512639</v>
+        <v>1.00539565310765</v>
       </c>
       <c r="M7" s="10" t="str">
         <f ca="1"/>
@@ -4334,7 +4334,7 @@
       </c>
       <c r="N7" s="128">
         <f ca="1"/>
-        <v>100.50961270637848</v>
+        <v>100.51753376835751</v>
       </c>
       <c r="O7" s="10" t="str">
         <f ca="1"/>
@@ -4342,7 +4342,7 @@
       </c>
       <c r="P7" s="118">
         <f ca="1"/>
-        <v>4.9226172101913879E-2</v>
+        <v>4.9252746987900338E-2</v>
       </c>
       <c r="Q7" s="20" t="str">
         <f ca="1"/>
@@ -4382,7 +4382,7 @@
     <row r="8" spans="1:26">
       <c r="A8" s="13" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.22/11/2025</v>
+        <v>AUD-Bond-AGB.0.04.12/12/2025</v>
       </c>
       <c r="B8" s="13" t="str">
         <f t="shared" si="0"/>
@@ -4396,7 +4396,7 @@
       </c>
       <c r="E8" s="83">
         <f t="shared" ca="1" si="1"/>
-        <v>45983</v>
+        <v>46003</v>
       </c>
       <c r="F8" s="36">
         <v>0.04</v>
@@ -4408,7 +4408,7 @@
       <c r="I8" s="18"/>
       <c r="J8" s="19" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.22/11/2025</v>
+        <v>AUD-Bond-AGB.0.04.12/12/2025</v>
       </c>
       <c r="K8" s="10" t="str">
         <f ca="1"/>
@@ -4416,7 +4416,7 @@
       </c>
       <c r="L8" s="38">
         <f ca="1"/>
-        <v>1.00161564837228</v>
+        <v>1.0015161032178801</v>
       </c>
       <c r="M8" s="10" t="str">
         <f ca="1"/>
@@ -4424,7 +4424,7 @@
       </c>
       <c r="N8" s="128">
         <f ca="1"/>
-        <v>100.13961612722022</v>
+        <v>100.12966379314365</v>
       </c>
       <c r="O8" s="10" t="str">
         <f ca="1"/>
@@ -4432,7 +4432,7 @@
       </c>
       <c r="P8" s="118">
         <f ca="1"/>
-        <v>5.6882314839381963E-2</v>
+        <v>5.685377170907991E-2</v>
       </c>
       <c r="Q8" s="20" t="str">
         <f ca="1"/>
@@ -4472,7 +4472,7 @@
     <row r="9" spans="1:26">
       <c r="A9" s="13" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.27/12/2026</v>
+        <v>AUD-Bond-AGB.0.04.16/01/2027</v>
       </c>
       <c r="B9" s="13" t="str">
         <f t="shared" si="0"/>
@@ -4486,7 +4486,7 @@
       </c>
       <c r="E9" s="83">
         <f t="shared" ca="1" si="1"/>
-        <v>46383</v>
+        <v>46403</v>
       </c>
       <c r="F9" s="36">
         <v>0.04</v>
@@ -4498,7 +4498,7 @@
       <c r="I9" s="18"/>
       <c r="J9" s="19" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.27/12/2026</v>
+        <v>AUD-Bond-AGB.0.04.16/01/2027</v>
       </c>
       <c r="K9" s="10" t="str">
         <f ca="1"/>
@@ -4506,7 +4506,7 @@
       </c>
       <c r="L9" s="38">
         <f ca="1"/>
-        <v>1.0176720437032101</v>
+        <v>1.0177705417429499</v>
       </c>
       <c r="M9" s="10" t="str">
         <f ca="1"/>
@@ -4514,7 +4514,7 @@
       </c>
       <c r="N9" s="128">
         <f ca="1"/>
-        <v>101.74490381161212</v>
+        <v>101.75475145716845</v>
       </c>
       <c r="O9" s="10" t="str">
         <f ca="1"/>
@@ -4522,7 +4522,7 @@
       </c>
       <c r="P9" s="118">
         <f ca="1"/>
-        <v>6.9094148293932178E-2</v>
+        <v>6.9096879258069052E-2</v>
       </c>
       <c r="Q9" s="20" t="str">
         <f ca="1"/>
@@ -4562,7 +4562,7 @@
     <row r="10" spans="1:26">
       <c r="A10" s="13" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.31/01/2028</v>
+        <v>AUD-Bond-AGB.0.04.20/02/2028</v>
       </c>
       <c r="B10" s="13" t="str">
         <f t="shared" si="0"/>
@@ -4576,7 +4576,7 @@
       </c>
       <c r="E10" s="83">
         <f t="shared" ca="1" si="1"/>
-        <v>46783</v>
+        <v>46803</v>
       </c>
       <c r="F10" s="36">
         <v>0.04</v>
@@ -4588,7 +4588,7 @@
       <c r="I10" s="18"/>
       <c r="J10" s="19" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.31/01/2028</v>
+        <v>AUD-Bond-AGB.0.04.20/02/2028</v>
       </c>
       <c r="K10" s="10" t="str">
         <f ca="1"/>
@@ -4612,7 +4612,7 @@
       </c>
       <c r="P10" s="118">
         <f ca="1"/>
-        <v>7.6008949096342496E-2</v>
+        <v>7.6000770358030406E-2</v>
       </c>
       <c r="Q10" s="20" t="str">
         <f ca="1"/>
@@ -4652,7 +4652,7 @@
     <row r="11" spans="1:26">
       <c r="A11" s="13" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.6/03/2029</v>
+        <v>AUD-Bond-AGB.0.04.26/03/2029</v>
       </c>
       <c r="B11" s="13" t="str">
         <f t="shared" si="0"/>
@@ -4666,7 +4666,7 @@
       </c>
       <c r="E11" s="83">
         <f t="shared" ca="1" si="1"/>
-        <v>47183</v>
+        <v>47203</v>
       </c>
       <c r="F11" s="36">
         <v>0.04</v>
@@ -4678,7 +4678,7 @@
       <c r="I11" s="18"/>
       <c r="J11" s="19" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.6/03/2029</v>
+        <v>AUD-Bond-AGB.0.04.26/03/2029</v>
       </c>
       <c r="K11" s="10" t="str">
         <f ca="1"/>
@@ -4702,7 +4702,7 @@
       </c>
       <c r="P11" s="118">
         <f ca="1"/>
-        <v>8.2601629578798144E-2</v>
+        <v>8.2599596219098098E-2</v>
       </c>
       <c r="Q11" s="20" t="str">
         <f ca="1"/>
@@ -4742,7 +4742,7 @@
     <row r="12" spans="1:26">
       <c r="A12" s="13" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.10/04/2030</v>
+        <v>AUD-Bond-AGB.0.04.30/04/2030</v>
       </c>
       <c r="B12" s="13" t="str">
         <f t="shared" si="0"/>
@@ -4756,7 +4756,7 @@
       </c>
       <c r="E12" s="83">
         <f t="shared" ca="1" si="1"/>
-        <v>47583</v>
+        <v>47603</v>
       </c>
       <c r="F12" s="36">
         <v>0.04</v>
@@ -4768,7 +4768,7 @@
       <c r="I12" s="18"/>
       <c r="J12" s="19" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.10/04/2030</v>
+        <v>AUD-Bond-AGB.0.04.30/04/2030</v>
       </c>
       <c r="K12" s="10" t="str">
         <f ca="1"/>
@@ -4792,7 +4792,7 @@
       </c>
       <c r="P12" s="118">
         <f ca="1"/>
-        <v>8.8855473217548359E-2</v>
+        <v>8.88656935434948E-2</v>
       </c>
       <c r="Q12" s="20" t="str">
         <f ca="1"/>
@@ -4832,7 +4832,7 @@
     <row r="13" spans="1:26">
       <c r="A13" s="13" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.15/05/2031</v>
+        <v>AUD-Bond-AGB.0.04.4/06/2031</v>
       </c>
       <c r="B13" s="13" t="str">
         <f t="shared" si="0"/>
@@ -4846,7 +4846,7 @@
       </c>
       <c r="E13" s="83">
         <f t="shared" ca="1" si="1"/>
-        <v>47983</v>
+        <v>48003</v>
       </c>
       <c r="F13" s="36">
         <v>0.04</v>
@@ -4858,7 +4858,7 @@
       <c r="I13" s="18"/>
       <c r="J13" s="19" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.15/05/2031</v>
+        <v>AUD-Bond-AGB.0.04.4/06/2031</v>
       </c>
       <c r="K13" s="10" t="str">
         <f ca="1"/>
@@ -4866,7 +4866,7 @@
       </c>
       <c r="L13" s="38">
         <f ca="1"/>
-        <v>1.00237051066565</v>
+        <v>1.0023834797009601</v>
       </c>
       <c r="M13" s="10" t="str">
         <f ca="1"/>
@@ -4874,7 +4874,7 @@
       </c>
       <c r="N13" s="128">
         <f ca="1"/>
-        <v>100.21508581502896</v>
+        <v>100.21638243436553</v>
       </c>
       <c r="O13" s="10" t="str">
         <f ca="1"/>
@@ -4882,7 +4882,7 @@
       </c>
       <c r="P13" s="118">
         <f ca="1"/>
-        <v>9.4813454129314897E-2</v>
+        <v>9.4813588229457096E-2</v>
       </c>
       <c r="Q13" s="20" t="str">
         <f ca="1"/>
@@ -4922,7 +4922,7 @@
     <row r="14" spans="1:26">
       <c r="A14" s="13" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.17/06/2032</v>
+        <v>AUD-Bond-AGB.0.04.7/07/2032</v>
       </c>
       <c r="B14" s="13" t="str">
         <f t="shared" si="0"/>
@@ -4936,7 +4936,7 @@
       </c>
       <c r="E14" s="83">
         <f ca="1">E13+399</f>
-        <v>48382</v>
+        <v>48402</v>
       </c>
       <c r="F14" s="36">
         <v>0.04</v>
@@ -4948,7 +4948,7 @@
       <c r="I14" s="18"/>
       <c r="J14" s="19" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.17/06/2032</v>
+        <v>AUD-Bond-AGB.0.04.7/07/2032</v>
       </c>
       <c r="K14" s="10" t="str">
         <f ca="1"/>
@@ -4956,7 +4956,7 @@
       </c>
       <c r="L14" s="38">
         <f ca="1"/>
-        <v>1.01877993094173</v>
+        <v>1.0187731942840199</v>
       </c>
       <c r="M14" s="10" t="str">
         <f ca="1"/>
@@ -4964,7 +4964,7 @@
       </c>
       <c r="N14" s="128">
         <f ca="1"/>
-        <v>101.85566825799225</v>
+        <v>101.85499473984369</v>
       </c>
       <c r="O14" s="10" t="str">
         <f ca="1"/>
@@ -4972,7 +4972,7 @@
       </c>
       <c r="P14" s="118">
         <f ca="1"/>
-        <v>0.10549556075384504</v>
+        <v>0.10546812891815011</v>
       </c>
       <c r="Q14" s="20" t="str">
         <f ca="1"/>
@@ -5012,7 +5012,7 @@
     <row r="15" spans="1:26">
       <c r="A15" s="13" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.22/07/2033</v>
+        <v>AUD-Bond-AGB.0.04.11/08/2033</v>
       </c>
       <c r="B15" s="13" t="str">
         <f t="shared" si="0"/>
@@ -5026,7 +5026,7 @@
       </c>
       <c r="E15" s="83">
         <f t="shared" ca="1" si="1"/>
-        <v>48782</v>
+        <v>48802</v>
       </c>
       <c r="F15" s="36">
         <v>0.04</v>
@@ -5038,7 +5038,7 @@
       <c r="I15" s="18"/>
       <c r="J15" s="19" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.22/07/2033</v>
+        <v>AUD-Bond-AGB.0.04.11/08/2033</v>
       </c>
       <c r="K15" s="10" t="str">
         <f ca="1"/>
@@ -5062,7 +5062,7 @@
       </c>
       <c r="P15" s="118">
         <f ca="1"/>
-        <v>0.11083595989690487</v>
+        <v>0.11083715388692164</v>
       </c>
       <c r="Q15" s="20" t="str">
         <f ca="1"/>
@@ -5102,7 +5102,7 @@
     <row r="16" spans="1:26">
       <c r="A16" s="13" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.26/08/2034</v>
+        <v>AUD-Bond-AGB.0.04.15/09/2034</v>
       </c>
       <c r="B16" s="13" t="str">
         <f t="shared" si="0"/>
@@ -5116,7 +5116,7 @@
       </c>
       <c r="E16" s="83">
         <f t="shared" ca="1" si="1"/>
-        <v>49182</v>
+        <v>49202</v>
       </c>
       <c r="F16" s="36">
         <v>0.04</v>
@@ -5128,7 +5128,7 @@
       <c r="I16" s="18"/>
       <c r="J16" s="19" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.26/08/2034</v>
+        <v>AUD-Bond-AGB.0.04.15/09/2034</v>
       </c>
       <c r="K16" s="10" t="str">
         <f ca="1"/>
@@ -5136,7 +5136,7 @@
       </c>
       <c r="L16" s="38">
         <f ca="1"/>
-        <v>1.0110007461444099</v>
+        <v>1.0111468344800201</v>
       </c>
       <c r="M16" s="10" t="str">
         <f ca="1"/>
@@ -5144,7 +5144,7 @@
       </c>
       <c r="N16" s="128">
         <f ca="1"/>
-        <v>101.07792024591569</v>
+        <v>101.0925258781983</v>
       </c>
       <c r="O16" s="10" t="str">
         <f ca="1"/>
@@ -5152,7 +5152,7 @@
       </c>
       <c r="P16" s="118">
         <f ca="1"/>
-        <v>0.11593876086417822</v>
+        <v>0.11602175714134967</v>
       </c>
       <c r="Q16" s="20" t="str">
         <f ca="1"/>
@@ -5192,7 +5192,7 @@
     <row r="17" spans="1:26">
       <c r="A17" s="13" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.30/09/2035</v>
+        <v>AUD-Bond-AGB.0.04.20/10/2035</v>
       </c>
       <c r="B17" s="13" t="str">
         <f t="shared" si="0"/>
@@ -5206,7 +5206,7 @@
       </c>
       <c r="E17" s="83">
         <f t="shared" ca="1" si="1"/>
-        <v>49582</v>
+        <v>49602</v>
       </c>
       <c r="F17" s="36">
         <v>0.04</v>
@@ -5218,7 +5218,7 @@
       <c r="I17" s="18"/>
       <c r="J17" s="19" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.30/09/2035</v>
+        <v>AUD-Bond-AGB.0.04.20/10/2035</v>
       </c>
       <c r="K17" s="10" t="str">
         <f ca="1"/>
@@ -5226,7 +5226,7 @@
       </c>
       <c r="L17" s="38">
         <f ca="1"/>
-        <v>1.00734520692108</v>
+        <v>1.0072764881473799</v>
       </c>
       <c r="M17" s="10" t="str">
         <f ca="1"/>
@@ -5234,7 +5234,7 @@
       </c>
       <c r="N17" s="128">
         <f ca="1"/>
-        <v>100.71244642853159</v>
+        <v>100.70557605701708</v>
       </c>
       <c r="O17" s="10" t="str">
         <f ca="1"/>
@@ -5242,7 +5242,7 @@
       </c>
       <c r="P17" s="118">
         <f ca="1"/>
-        <v>0.12087885757594044</v>
+        <v>0.12084291079916384</v>
       </c>
       <c r="Q17" s="20" t="str">
         <f ca="1"/>
@@ -5282,7 +5282,7 @@
     <row r="18" spans="1:26">
       <c r="A18" s="13" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.3/11/2036</v>
+        <v>AUD-Bond-AGB.0.04.23/11/2036</v>
       </c>
       <c r="B18" s="13" t="str">
         <f t="shared" si="0"/>
@@ -5296,7 +5296,7 @@
       </c>
       <c r="E18" s="83">
         <f t="shared" ca="1" si="1"/>
-        <v>49982</v>
+        <v>50002</v>
       </c>
       <c r="F18" s="36">
         <v>0.04</v>
@@ -5308,7 +5308,7 @@
       <c r="I18" s="18"/>
       <c r="J18" s="19" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.3/11/2036</v>
+        <v>AUD-Bond-AGB.0.04.23/11/2036</v>
       </c>
       <c r="K18" s="10" t="str">
         <f ca="1"/>
@@ -5332,7 +5332,7 @@
       </c>
       <c r="P18" s="118">
         <f ca="1"/>
-        <v>0.12550342756962579</v>
+        <v>0.12550243992611027</v>
       </c>
       <c r="Q18" s="20" t="str">
         <f ca="1"/>
@@ -5372,7 +5372,7 @@
     <row r="19" spans="1:26">
       <c r="A19" s="13" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.8/12/2037</v>
+        <v>AUD-Bond-AGB.0.04.28/12/2037</v>
       </c>
       <c r="B19" s="13" t="str">
         <f t="shared" si="0"/>
@@ -5386,7 +5386,7 @@
       </c>
       <c r="E19" s="83">
         <f t="shared" ca="1" si="1"/>
-        <v>50382</v>
+        <v>50402</v>
       </c>
       <c r="F19" s="36">
         <v>0.04</v>
@@ -5398,7 +5398,7 @@
       <c r="I19" s="18"/>
       <c r="J19" s="19" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.8/12/2037</v>
+        <v>AUD-Bond-AGB.0.04.28/12/2037</v>
       </c>
       <c r="K19" s="10" t="str">
         <f ca="1"/>
@@ -5422,7 +5422,7 @@
       </c>
       <c r="P19" s="118">
         <f ca="1"/>
-        <v>0.13483017534937086</v>
+        <v>0.13483092101592969</v>
       </c>
       <c r="Q19" s="20" t="str">
         <f ca="1"/>
@@ -5462,7 +5462,7 @@
     <row r="20" spans="1:26">
       <c r="A20" s="13" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.12/01/2039</v>
+        <v>AUD-Bond-AGB.0.04.1/02/2039</v>
       </c>
       <c r="B20" s="13" t="str">
         <f t="shared" si="0"/>
@@ -5476,7 +5476,7 @@
       </c>
       <c r="E20" s="83">
         <f t="shared" ca="1" si="1"/>
-        <v>50782</v>
+        <v>50802</v>
       </c>
       <c r="F20" s="36">
         <v>0.04</v>
@@ -5488,7 +5488,7 @@
       <c r="I20" s="18"/>
       <c r="J20" s="19" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.12/01/2039</v>
+        <v>AUD-Bond-AGB.0.04.1/02/2039</v>
       </c>
       <c r="K20" s="10" t="str">
         <f ca="1"/>
@@ -5512,7 +5512,7 @@
       </c>
       <c r="P20" s="118">
         <f ca="1"/>
-        <v>0.13896645435225971</v>
+        <v>0.13896158730756458</v>
       </c>
       <c r="Q20" s="20" t="str">
         <f ca="1"/>
@@ -5552,7 +5552,7 @@
     <row r="21" spans="1:26">
       <c r="A21" s="13" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.16/02/2040</v>
+        <v>AUD-Bond-AGB.0.04.7/03/2040</v>
       </c>
       <c r="B21" s="13" t="str">
         <f t="shared" si="0"/>
@@ -5566,7 +5566,7 @@
       </c>
       <c r="E21" s="83">
         <f t="shared" ca="1" si="1"/>
-        <v>51182</v>
+        <v>51202</v>
       </c>
       <c r="F21" s="36">
         <v>0.04</v>
@@ -5578,7 +5578,7 @@
       <c r="I21" s="18"/>
       <c r="J21" s="19" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.16/02/2040</v>
+        <v>AUD-Bond-AGB.0.04.7/03/2040</v>
       </c>
       <c r="K21" s="10" t="str">
         <f ca="1"/>
@@ -5586,7 +5586,7 @@
       </c>
       <c r="L21" s="38">
         <f ca="1"/>
-        <v>1.0121074548097999</v>
+        <v>1.01201779040503</v>
       </c>
       <c r="M21" s="10" t="str">
         <f ca="1"/>
@@ -5594,7 +5594,7 @@
       </c>
       <c r="N21" s="128">
         <f ca="1"/>
-        <v>101.18856686080925</v>
+        <v>101.17960238517577</v>
       </c>
       <c r="O21" s="10" t="str">
         <f ca="1"/>
@@ -5602,7 +5602,7 @@
       </c>
       <c r="P21" s="118">
         <f ca="1"/>
-        <v>0.1428859075967652</v>
+        <v>0.14291146326999876</v>
       </c>
       <c r="Q21" s="20" t="str">
         <f ca="1"/>
@@ -5642,7 +5642,7 @@
     <row r="22" spans="1:26">
       <c r="A22" s="13" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.22/03/2041</v>
+        <v>AUD-Bond-AGB.0.04.11/04/2041</v>
       </c>
       <c r="B22" s="13" t="str">
         <f t="shared" si="0"/>
@@ -5656,7 +5656,7 @@
       </c>
       <c r="E22" s="83">
         <f t="shared" ca="1" si="1"/>
-        <v>51582</v>
+        <v>51602</v>
       </c>
       <c r="F22" s="36">
         <v>0.04</v>
@@ -5668,7 +5668,7 @@
       <c r="I22" s="18"/>
       <c r="J22" s="19" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.22/03/2041</v>
+        <v>AUD-Bond-AGB.0.04.11/04/2041</v>
       </c>
       <c r="K22" s="10" t="str">
         <f ca="1"/>
@@ -5676,7 +5676,7 @@
       </c>
       <c r="L22" s="38">
         <f ca="1"/>
-        <v>1.0082128882968999</v>
+        <v>1.00825795226635</v>
       </c>
       <c r="M22" s="10" t="str">
         <f ca="1"/>
@@ -5684,7 +5684,7 @@
       </c>
       <c r="N22" s="128">
         <f ca="1"/>
-        <v>100.79919555234626</v>
+        <v>100.80370096179071</v>
       </c>
       <c r="O22" s="10" t="str">
         <f ca="1"/>
@@ -5692,7 +5692,7 @@
       </c>
       <c r="P22" s="118">
         <f ca="1"/>
-        <v>0.14662808581826764</v>
+        <v>0.14662450364581689</v>
       </c>
       <c r="Q22" s="20" t="str">
         <f ca="1"/>
@@ -6138,11 +6138,11 @@
       </c>
       <c r="B38" s="106">
         <f ca="1">AUDCurve!C4</f>
-        <v>43620.688124768516</v>
+        <v>43640.48577013889</v>
       </c>
       <c r="D38" s="6">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetBondAssetSwapSpread(A2, B38, B39, B40, E2, B43, F2, B42, B41, B37, B44, B45, G2, B36)</f>
-        <v>-2.1051484339508375E-4</v>
+        <v>-1.8122058298947419E-4</v>
       </c>
       <c r="H38" s="6" t="str">
         <v>NPV</v>
@@ -6182,14 +6182,14 @@
       </c>
       <c r="B39" s="106">
         <f ca="1">B38+3</f>
-        <v>43623.688124768516</v>
+        <v>43643.48577013889</v>
       </c>
       <c r="H39" s="6" t="str">
         <v>AccruedInterest</v>
       </c>
       <c r="J39" s="120" t="str">
         <f t="array" aca="1" ref="J39:U58" ca="1">_xll.HLV5r3.Financial.Cache.EvaluateMetricsRawData( $H$2:$H$7, $B$36, A3:A22, $B$38)</f>
-        <v>AUD-Bond-AGB.0.04.1/06/2020</v>
+        <v>AUD-Bond-AGB.0.04.21/06/2020</v>
       </c>
       <c r="K39" s="123" t="str">
         <f ca="1"/>
@@ -6251,7 +6251,7 @@
       </c>
       <c r="J40" s="121" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.1/06/2020</v>
+        <v>AUD-Bond-AGB.0.04.21/06/2020</v>
       </c>
       <c r="K40" s="124" t="str">
         <f ca="1"/>
@@ -6313,7 +6313,7 @@
       </c>
       <c r="J41" s="121" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.1/06/2020</v>
+        <v>AUD-Bond-AGB.0.04.21/06/2020</v>
       </c>
       <c r="K41" s="124" t="str">
         <f ca="1"/>
@@ -6321,7 +6321,7 @@
       </c>
       <c r="L41" s="38">
         <f ca="1"/>
-        <v>9.7348357975800652E-3</v>
+        <v>9.7337164492171183E-3</v>
       </c>
       <c r="M41" s="10" t="e">
         <f ca="1"/>
@@ -6375,7 +6375,7 @@
       </c>
       <c r="J42" s="121" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.1/06/2020</v>
+        <v>AUD-Bond-AGB.0.04.21/06/2020</v>
       </c>
       <c r="K42" s="124" t="str">
         <f ca="1"/>
@@ -6383,7 +6383,7 @@
       </c>
       <c r="L42" s="38">
         <f ca="1"/>
-        <v>-1.9621107309635808E-4</v>
+        <v>-3.1432539804813456E-4</v>
       </c>
       <c r="M42" s="10" t="e">
         <f ca="1"/>
@@ -6437,7 +6437,7 @@
       </c>
       <c r="J43" s="121" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.6/07/2021</v>
+        <v>AUD-Bond-AGB.0.04.26/07/2021</v>
       </c>
       <c r="K43" s="124" t="str">
         <f ca="1"/>
@@ -6499,7 +6499,7 @@
       </c>
       <c r="J44" s="121" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.6/07/2021</v>
+        <v>AUD-Bond-AGB.0.04.26/07/2021</v>
       </c>
       <c r="K44" s="124" t="str">
         <f ca="1"/>
@@ -6561,7 +6561,7 @@
       </c>
       <c r="J45" s="121" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.6/07/2021</v>
+        <v>AUD-Bond-AGB.0.04.26/07/2021</v>
       </c>
       <c r="K45" s="124" t="str">
         <f ca="1"/>
@@ -6569,7 +6569,7 @@
       </c>
       <c r="L45" s="38">
         <f ca="1"/>
-        <v>2.3933118071269927E-2</v>
+        <v>2.3932000570792946E-2</v>
       </c>
       <c r="M45" s="10" t="e">
         <f ca="1"/>
@@ -6617,7 +6617,7 @@
       </c>
       <c r="J46" s="121" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.6/07/2021</v>
+        <v>AUD-Bond-AGB.0.04.26/07/2021</v>
       </c>
       <c r="K46" s="124" t="str">
         <f ca="1"/>
@@ -6625,7 +6625,7 @@
       </c>
       <c r="L46" s="38">
         <f ca="1"/>
-        <v>-2.1166962535973128E-4</v>
+        <v>-2.1360252292045785E-4</v>
       </c>
       <c r="M46" s="10" t="e">
         <f ca="1"/>
@@ -6673,7 +6673,7 @@
       </c>
       <c r="J47" s="121" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.10/08/2022</v>
+        <v>AUD-Bond-AGB.0.04.30/08/2022</v>
       </c>
       <c r="K47" s="124" t="str">
         <f ca="1"/>
@@ -6681,7 +6681,7 @@
       </c>
       <c r="L47" s="38">
         <f ca="1"/>
-        <v>1.0127720614331199</v>
+        <v>1.0128507778089599</v>
       </c>
       <c r="M47" s="10" t="e">
         <f ca="1"/>
@@ -6729,7 +6729,7 @@
       </c>
       <c r="J48" s="121" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.10/08/2022</v>
+        <v>AUD-Bond-AGB.0.04.30/08/2022</v>
       </c>
       <c r="K48" s="124" t="str">
         <f ca="1"/>
@@ -6737,7 +6737,7 @@
       </c>
       <c r="L48" s="38">
         <f ca="1"/>
-        <v>101.25501295941307</v>
+        <v>101.26288287206106</v>
       </c>
       <c r="M48" s="10" t="e">
         <f ca="1"/>
@@ -6785,7 +6785,7 @@
       </c>
       <c r="J49" s="121" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.10/08/2022</v>
+        <v>AUD-Bond-AGB.0.04.30/08/2022</v>
       </c>
       <c r="K49" s="124" t="str">
         <f ca="1"/>
@@ -6793,7 +6793,7 @@
       </c>
       <c r="L49" s="38">
         <f ca="1"/>
-        <v>3.2740001264981632E-2</v>
+        <v>3.2796514448903885E-2</v>
       </c>
       <c r="M49" s="10" t="e">
         <f ca="1"/>
@@ -6838,7 +6838,7 @@
     <row r="50" spans="8:24">
       <c r="J50" s="121" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.10/08/2022</v>
+        <v>AUD-Bond-AGB.0.04.30/08/2022</v>
       </c>
       <c r="K50" s="124" t="str">
         <f ca="1"/>
@@ -6846,7 +6846,7 @@
       </c>
       <c r="L50" s="38">
         <f ca="1"/>
-        <v>-1.8115544065193577E-4</v>
+        <v>-1.3604615500413983E-4</v>
       </c>
       <c r="M50" s="10" t="e">
         <f ca="1"/>
@@ -6891,7 +6891,7 @@
     <row r="51" spans="8:24">
       <c r="J51" s="121" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.14/09/2023</v>
+        <v>AUD-Bond-AGB.0.04.4/10/2023</v>
       </c>
       <c r="K51" s="124" t="str">
         <f ca="1"/>
@@ -6899,7 +6899,7 @@
       </c>
       <c r="L51" s="38">
         <f ca="1"/>
-        <v>1.00908131705403</v>
+        <v>1.0090219743548801</v>
       </c>
       <c r="M51" s="10" t="e">
         <f ca="1"/>
@@ -6944,7 +6944,7 @@
     <row r="52" spans="8:24">
       <c r="J52" s="121" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.14/09/2023</v>
+        <v>AUD-Bond-AGB.0.04.4/10/2023</v>
       </c>
       <c r="K52" s="124" t="str">
         <f ca="1"/>
@@ -6952,7 +6952,7 @@
       </c>
       <c r="L52" s="38">
         <f ca="1"/>
-        <v>100.88601939791432</v>
+        <v>100.88008642839404</v>
       </c>
       <c r="M52" s="10" t="e">
         <f ca="1"/>
@@ -6997,7 +6997,7 @@
     <row r="53" spans="8:24">
       <c r="J53" s="121" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.14/09/2023</v>
+        <v>AUD-Bond-AGB.0.04.4/10/2023</v>
       </c>
       <c r="K53" s="124" t="str">
         <f ca="1"/>
@@ -7005,7 +7005,7 @@
       </c>
       <c r="L53" s="38">
         <f ca="1"/>
-        <v>4.1219483287832544E-2</v>
+        <v>4.1191409225107611E-2</v>
       </c>
       <c r="M53" s="10" t="e">
         <f ca="1"/>
@@ -7050,7 +7050,7 @@
     <row r="54" spans="8:24">
       <c r="J54" s="121" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.14/09/2023</v>
+        <v>AUD-Bond-AGB.0.04.4/10/2023</v>
       </c>
       <c r="K54" s="124" t="str">
         <f ca="1"/>
@@ -7058,7 +7058,7 @@
       </c>
       <c r="L54" s="38">
         <f ca="1"/>
-        <v>1.5585295155031499E-5</v>
+        <v>3.1312201725133846E-6</v>
       </c>
       <c r="M54" s="10" t="e">
         <f ca="1"/>
@@ -7103,7 +7103,7 @@
     <row r="55" spans="8:24">
       <c r="J55" s="121" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.18/10/2024</v>
+        <v>AUD-Bond-AGB.0.04.7/11/2024</v>
       </c>
       <c r="K55" s="124" t="str">
         <f ca="1"/>
@@ -7111,7 +7111,7 @@
       </c>
       <c r="L55" s="38">
         <f ca="1"/>
-        <v>1.00531642512639</v>
+        <v>1.00539565310765</v>
       </c>
       <c r="M55" s="10" t="e">
         <f ca="1"/>
@@ -7156,7 +7156,7 @@
     <row r="56" spans="8:24">
       <c r="J56" s="121" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.18/10/2024</v>
+        <v>AUD-Bond-AGB.0.04.7/11/2024</v>
       </c>
       <c r="K56" s="124" t="str">
         <f ca="1"/>
@@ -7164,7 +7164,7 @@
       </c>
       <c r="L56" s="38">
         <f ca="1"/>
-        <v>100.50961270637848</v>
+        <v>100.51753376835751</v>
       </c>
       <c r="M56" s="10" t="e">
         <f ca="1"/>
@@ -7209,7 +7209,7 @@
     <row r="57" spans="8:24">
       <c r="J57" s="121" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.18/10/2024</v>
+        <v>AUD-Bond-AGB.0.04.7/11/2024</v>
       </c>
       <c r="K57" s="124" t="str">
         <f ca="1"/>
@@ -7217,7 +7217,7 @@
       </c>
       <c r="L57" s="38">
         <f ca="1"/>
-        <v>4.9226172101913879E-2</v>
+        <v>4.9252746987900338E-2</v>
       </c>
       <c r="M57" s="10" t="e">
         <f ca="1"/>
@@ -7262,7 +7262,7 @@
     <row r="58" spans="8:24">
       <c r="J58" s="121" t="str">
         <f ca="1"/>
-        <v>AUD-Bond-AGB.0.04.18/10/2024</v>
+        <v>AUD-Bond-AGB.0.04.7/11/2024</v>
       </c>
       <c r="K58" s="124" t="str">
         <f ca="1"/>
@@ -7270,7 +7270,7 @@
       </c>
       <c r="L58" s="38">
         <f ca="1"/>
-        <v>1.0377767056683269E-6</v>
+        <v>6.730465234044659E-6</v>
       </c>
       <c r="M58" s="10" t="e">
         <f ca="1"/>

</xml_diff>